<commit_message>
dir. merged cells solved
</commit_message>
<xml_diff>
--- a/Movies_New_Record.xlsx
+++ b/Movies_New_Record.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ECA681-225A-41DD-8C01-F60F79DF6331}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADAA3F23-FC41-490A-AF88-2607F3017845}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -246,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -254,36 +254,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -309,11 +317,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,161 +802,160 @@
   <dimension ref="C1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:R5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="3" customWidth="1"/>
-    <col min="9" max="10" width="11.140625" style="3" customWidth="1"/>
-    <col min="11" max="13" width="9.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="3" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="3" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="2" width="9.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="14" style="9" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="9" customWidth="1"/>
+    <col min="11" max="13" width="9.140625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="14.7109375" style="9" customWidth="1"/>
+    <col min="15" max="28" width="9.140625" style="9" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="6"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="20" t="s">
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="R1" s="21"/>
+      <c r="R1" s="25"/>
     </row>
     <row r="2" spans="3:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="10" t="s">
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="10" t="s">
+      <c r="L2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="10" t="s">
+      <c r="M2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="10" t="s">
+      <c r="N2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="10" t="s">
+      <c r="O2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="10" t="s">
+      <c r="P2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="10" t="s">
+      <c r="Q2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="R2" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="3:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="24"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="20"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="3:18" x14ac:dyDescent="0.25">
-      <c r="C4" s="25"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="18"/>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="18"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="3:18" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="26"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="19"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
       <c r="R5" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="D3:D5"/>
-    <mergeCell ref="E3:E5"/>
-    <mergeCell ref="F3:F5"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="J3:J5"/>
+  <mergeCells count="11">
     <mergeCell ref="N3:N5"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="K1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="H2:J2"/>
     <mergeCell ref="I3:I5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="D3:D5"/>
+    <mergeCell ref="E3:E5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="J3:J5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H3:J5" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>